<commit_message>
create service for generate excel using jdbcTemplate
</commit_message>
<xml_diff>
--- a/example-result-download/GenerateExcelUsingList.xlsx
+++ b/example-result-download/GenerateExcelUsingList.xlsx
@@ -359,13 +359,13 @@
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Total data</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t xml:space="preserve"> : 6</t>
         </is>

</xml_diff>